<commit_message>
Criação do CSV quase funcionando
</commit_message>
<xml_diff>
--- a/teste2.xlsx
+++ b/teste2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computador\OneDrive\Faculdade\OITAVO SEMESTRE\Estágio\aplicação\nova-api-estagio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C162E7FC-CA91-4DE8-ADC3-B353E4C35CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F649980-AA5E-4D8F-BCB8-C1B9F842B1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,7 +360,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>